<commit_message>
#130 negligible changes to analysis notebook
</commit_message>
<xml_diff>
--- a/src/technology/template/template.xlsx
+++ b/src/technology/template/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C95DB6-24B1-4A8F-856C-51732F4292CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1049331-2DC3-4861-89EB-E190E6254857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="6" xr2:uid="{277ED3FD-2B20-4A36-BB03-16AF83BDC75C}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{277ED3FD-2B20-4A36-BB03-16AF83BDC75C}"/>
   </bookViews>
   <sheets>
     <sheet name="indices" sheetId="1" r:id="rId1"/>
@@ -1162,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF3D170-DEC1-4938-B961-67DBF048922E}">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16910,7 +16910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD318B56-38BD-4E5D-86D7-782D60429334}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
#130 adds overall efficiency as a fourth metric
</commit_message>
<xml_diff>
--- a/src/technology/template/template.xlsx
+++ b/src/technology/template/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1049331-2DC3-4861-89EB-E190E6254857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3F87A8-332F-4770-8BEB-092FB6732105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{277ED3FD-2B20-4A36-BB03-16AF83BDC75C}"/>
+    <workbookView xWindow="33780" yWindow="0" windowWidth="20550" windowHeight="16200" activeTab="4" xr2:uid="{277ED3FD-2B20-4A36-BB03-16AF83BDC75C}"/>
   </bookViews>
   <sheets>
     <sheet name="indices" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">designs!$A$1:$G$421</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indices!$A$1:$F$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">indices!$A$1:$F$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">parameters!$A$1:$G$301</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3802" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3817" uniqueCount="256">
   <si>
     <t>Category</t>
   </si>
@@ -809,6 +809,12 @@
   </si>
   <si>
     <t>Component B2 Low Funding</t>
+  </si>
+  <si>
+    <t>It's important that all Metrics be calculable for all Technologies evaluated within a decision context, as Metrics are a key part of evaluating and comparing R&amp;D investments.</t>
+  </si>
+  <si>
+    <t>Overall Efficiency</t>
   </si>
 </sst>
 </file>
@@ -1160,17 +1166,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AF3D170-DEC1-4938-B961-67DBF048922E}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.28515625" bestFit="1" customWidth="1"/>
@@ -1367,22 +1373,22 @@
       <c r="D12">
         <v>2</v>
       </c>
+      <c r="F12" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>255</v>
       </c>
       <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1393,13 +1399,13 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1410,24 +1416,27 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>231</v>
+        <v>94</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1438,10 +1447,10 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1452,10 +1461,10 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1466,10 +1475,10 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>229</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1480,10 +1489,10 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1491,13 +1500,13 @@
         <v>91</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1508,10 +1517,10 @@
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1522,10 +1531,10 @@
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1533,13 +1542,13 @@
         <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1550,10 +1559,10 @@
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1564,10 +1573,10 @@
         <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1575,13 +1584,13 @@
         <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1589,13 +1598,13 @@
         <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>255</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1606,17 +1615,45 @@
         <v>12</v>
       </c>
       <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" t="s">
         <v>94</v>
       </c>
-      <c r="D29">
+      <c r="D31">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F29">
-    <sortCondition ref="A4:A29"/>
-    <sortCondition ref="B4:B29"/>
-    <sortCondition ref="D4:D29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:F31">
+    <sortCondition ref="A4:A31"/>
+    <sortCondition ref="B4:B31"/>
+    <sortCondition ref="D4:D31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16233,16 +16270,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08421A62-7A7F-4754-940E-DE21752714F2}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16378,16 +16415,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>255</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -16395,13 +16432,13 @@
         <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -16412,7 +16449,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
         <v>132</v>
@@ -16426,7 +16463,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
         <v>132</v>
@@ -16437,13 +16474,13 @@
         <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -16454,10 +16491,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -16468,10 +16505,38 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
         <v>41</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>255</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#130 changes box to violin plots; separates technology results
</commit_message>
<xml_diff>
--- a/src/technology/template/template.xlsx
+++ b/src/technology/template/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9A4A68-5D7D-4192-A660-8433574084E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB96854E-4694-4B9B-A3D0-28F1764CC22F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29415" yWindow="1035" windowWidth="24660" windowHeight="14040" activeTab="4" xr2:uid="{277ED3FD-2B20-4A36-BB03-16AF83BDC75C}"/>
+    <workbookView xWindow="29850" yWindow="1065" windowWidth="24660" windowHeight="14040" activeTab="2" xr2:uid="{277ED3FD-2B20-4A36-BB03-16AF83BDC75C}"/>
   </bookViews>
   <sheets>
     <sheet name="indices" sheetId="1" r:id="rId1"/>
@@ -1841,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB20890-62B7-47AF-BA68-650F053D99C5}">
   <dimension ref="A1:G421"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10292,7 +10292,7 @@
   <dimension ref="A1:G301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E294" sqref="E294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10504,7 +10504,7 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
         <v>148</v>
@@ -10840,7 +10840,7 @@
         <v>7</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F24" t="s">
         <v>148</v>
@@ -11140,7 +11140,7 @@
         <v>7</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F39" t="s">
         <v>148</v>
@@ -11440,7 +11440,7 @@
         <v>7</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F54" t="s">
         <v>148</v>
@@ -11740,7 +11740,7 @@
         <v>7</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F69" t="s">
         <v>148</v>
@@ -12040,7 +12040,7 @@
         <v>7</v>
       </c>
       <c r="E84">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F84" t="s">
         <v>148</v>
@@ -12340,7 +12340,7 @@
         <v>7</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F99" t="s">
         <v>148</v>
@@ -12640,7 +12640,7 @@
         <v>7</v>
       </c>
       <c r="E114">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F114" t="s">
         <v>148</v>
@@ -12940,7 +12940,7 @@
         <v>7</v>
       </c>
       <c r="E129">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F129" t="s">
         <v>148</v>
@@ -13240,7 +13240,7 @@
         <v>7</v>
       </c>
       <c r="E144">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F144" t="s">
         <v>148</v>
@@ -13500,7 +13500,7 @@
         <v>5</v>
       </c>
       <c r="E157">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F157" t="s">
         <v>148</v>
@@ -13803,7 +13803,7 @@
         <v>5</v>
       </c>
       <c r="E172">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F172" t="s">
         <v>148</v>
@@ -14106,7 +14106,7 @@
         <v>5</v>
       </c>
       <c r="E187">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F187" t="s">
         <v>148</v>
@@ -14406,7 +14406,7 @@
         <v>5</v>
       </c>
       <c r="E202">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F202" t="s">
         <v>148</v>
@@ -14706,7 +14706,7 @@
         <v>5</v>
       </c>
       <c r="E217">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F217" t="s">
         <v>148</v>
@@ -15006,7 +15006,7 @@
         <v>5</v>
       </c>
       <c r="E232">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F232" t="s">
         <v>148</v>
@@ -15306,7 +15306,7 @@
         <v>5</v>
       </c>
       <c r="E247">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F247" t="s">
         <v>148</v>
@@ -15606,7 +15606,7 @@
         <v>5</v>
       </c>
       <c r="E262">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F262" t="s">
         <v>148</v>
@@ -15906,7 +15906,7 @@
         <v>5</v>
       </c>
       <c r="E277">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F277" t="s">
         <v>148</v>
@@ -16206,7 +16206,7 @@
         <v>5</v>
       </c>
       <c r="E292">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F292" t="s">
         <v>148</v>
@@ -16406,7 +16406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08421A62-7A7F-4754-940E-DE21752714F2}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>

</xml_diff>